<commit_message>
Dodawanie większej ilości gier działa Czyszczenie exela takze Zostało dodawanie graczy i zeby wyswietlały sie ich imiona ;-;
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,10 +435,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>36</v>
-      </c>
-      <c r="C2" t="n">
         <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>28</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>